<commit_message>
exported updated V3 schematic PDF and BOM
</commit_message>
<xml_diff>
--- a/bici-pcb-BOM-V3.xlsx
+++ b/bici-pcb-BOM-V3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truth\OneDrive\Desktop\ACADEMICS\ENGN1650\engn1650-bici-pcb\bici-pcb\Project Outputs for bici-pcb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B83D3B55-D6F0-4A35-ADBA-C9E28C85FE72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9CD3A6F2-6F7A-4AB4-9872-00254F77AC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{51BD93EA-9FDD-4A87-A59D-4C51FA5BBC36}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{2C7AD2E0-6C97-4485-9083-9C9EA94C82E7}"/>
   </bookViews>
   <sheets>
     <sheet name="bici-pcb" sheetId="1" r:id="rId1"/>
@@ -122,6 +122,9 @@
     <t>C101, C201, C202, C402, C403, C404, C405</t>
   </si>
   <si>
+    <t>KYOCERA AVX</t>
+  </si>
+  <si>
     <t>478-KGM15AR70J104JTCT-ND</t>
   </si>
   <si>
@@ -150,9 +153,6 @@
   </si>
   <si>
     <t>C103</t>
-  </si>
-  <si>
-    <t>KYOCERA AVX</t>
   </si>
   <si>
     <t>478-KGM15AV51H103ZTCT-ND</t>
@@ -920,7 +920,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83C2E875-CDC3-4F55-BD40-5C9692D349B5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2150D750-15CD-4E4B-A8A1-C69239AC1EBD}">
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1042,7 +1042,7 @@
         <v>7</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>24</v>
@@ -1051,10 +1051,10 @@
         <v>14</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>17</v>
@@ -1062,13 +1062,13 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D5" s="1">
         <v>1</v>
@@ -1077,16 +1077,16 @@
         <v>21</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>17</v>
@@ -1094,22 +1094,22 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>14</v>

</xml_diff>